<commit_message>
Editing code and adding files from code, and adding better confusion matrix
</commit_message>
<xml_diff>
--- a/archive/duplicates.xlsx
+++ b/archive/duplicates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>length_url</t>
   </si>
@@ -275,6 +275,9 @@
   </si>
   <si>
     <t>page_rank</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -632,13 +635,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CJ175"/>
+  <dimension ref="A1:CK175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:88">
+    <row r="1" spans="1:89">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -900,8 +903,11 @@
       <c r="CJ1" s="1" t="s">
         <v>86</v>
       </c>
+      <c r="CK1" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
-    <row r="2" spans="1:88">
+    <row r="2" spans="1:89">
       <c r="A2" s="1">
         <v>1217</v>
       </c>
@@ -1166,8 +1172,11 @@
       <c r="CJ2">
         <v>6</v>
       </c>
+      <c r="CK2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:89">
       <c r="A3" s="1">
         <v>1480</v>
       </c>
@@ -1432,8 +1441,11 @@
       <c r="CJ3">
         <v>0</v>
       </c>
+      <c r="CK3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:88">
+    <row r="4" spans="1:89">
       <c r="A4" s="1">
         <v>1828</v>
       </c>
@@ -1698,8 +1710,11 @@
       <c r="CJ4">
         <v>5</v>
       </c>
+      <c r="CK4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:88">
+    <row r="5" spans="1:89">
       <c r="A5" s="1">
         <v>1948</v>
       </c>
@@ -1964,8 +1979,11 @@
       <c r="CJ5">
         <v>0</v>
       </c>
+      <c r="CK5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:88">
+    <row r="6" spans="1:89">
       <c r="A6" s="1">
         <v>2142</v>
       </c>
@@ -2230,8 +2248,11 @@
       <c r="CJ6">
         <v>0</v>
       </c>
+      <c r="CK6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:88">
+    <row r="7" spans="1:89">
       <c r="A7" s="1">
         <v>2229</v>
       </c>
@@ -2496,8 +2517,11 @@
       <c r="CJ7">
         <v>2</v>
       </c>
+      <c r="CK7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:88">
+    <row r="8" spans="1:89">
       <c r="A8" s="1">
         <v>2452</v>
       </c>
@@ -2762,8 +2786,11 @@
       <c r="CJ8">
         <v>5</v>
       </c>
+      <c r="CK8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:88">
+    <row r="9" spans="1:89">
       <c r="A9" s="1">
         <v>2463</v>
       </c>
@@ -3028,8 +3055,11 @@
       <c r="CJ9">
         <v>4</v>
       </c>
+      <c r="CK9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:88">
+    <row r="10" spans="1:89">
       <c r="A10" s="1">
         <v>2483</v>
       </c>
@@ -3294,8 +3324,11 @@
       <c r="CJ10">
         <v>5</v>
       </c>
+      <c r="CK10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:88">
+    <row r="11" spans="1:89">
       <c r="A11" s="1">
         <v>2682</v>
       </c>
@@ -3560,8 +3593,11 @@
       <c r="CJ11">
         <v>5</v>
       </c>
+      <c r="CK11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:88">
+    <row r="12" spans="1:89">
       <c r="A12" s="1">
         <v>2697</v>
       </c>
@@ -3826,8 +3862,11 @@
       <c r="CJ12">
         <v>0</v>
       </c>
+      <c r="CK12">
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:88">
+    <row r="13" spans="1:89">
       <c r="A13" s="1">
         <v>2717</v>
       </c>
@@ -4092,8 +4131,11 @@
       <c r="CJ13">
         <v>2</v>
       </c>
+      <c r="CK13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:88">
+    <row r="14" spans="1:89">
       <c r="A14" s="1">
         <v>2806</v>
       </c>
@@ -4358,8 +4400,11 @@
       <c r="CJ14">
         <v>5</v>
       </c>
+      <c r="CK14">
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:88">
+    <row r="15" spans="1:89">
       <c r="A15" s="1">
         <v>2869</v>
       </c>
@@ -4624,8 +4669,11 @@
       <c r="CJ15">
         <v>5</v>
       </c>
+      <c r="CK15">
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:88">
+    <row r="16" spans="1:89">
       <c r="A16" s="1">
         <v>2961</v>
       </c>
@@ -4890,8 +4938,11 @@
       <c r="CJ16">
         <v>0</v>
       </c>
+      <c r="CK16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:88">
+    <row r="17" spans="1:89">
       <c r="A17" s="1">
         <v>2995</v>
       </c>
@@ -5156,8 +5207,11 @@
       <c r="CJ17">
         <v>5</v>
       </c>
+      <c r="CK17">
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:88">
+    <row r="18" spans="1:89">
       <c r="A18" s="1">
         <v>3117</v>
       </c>
@@ -5422,8 +5476,11 @@
       <c r="CJ18">
         <v>5</v>
       </c>
+      <c r="CK18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:88">
+    <row r="19" spans="1:89">
       <c r="A19" s="1">
         <v>3181</v>
       </c>
@@ -5688,8 +5745,11 @@
       <c r="CJ19">
         <v>1</v>
       </c>
+      <c r="CK19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:88">
+    <row r="20" spans="1:89">
       <c r="A20" s="1">
         <v>3229</v>
       </c>
@@ -5954,8 +6014,11 @@
       <c r="CJ20">
         <v>0</v>
       </c>
+      <c r="CK20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="21" spans="1:88">
+    <row r="21" spans="1:89">
       <c r="A21" s="1">
         <v>3278</v>
       </c>
@@ -6220,8 +6283,11 @@
       <c r="CJ21">
         <v>5</v>
       </c>
+      <c r="CK21">
+        <v>0</v>
+      </c>
     </row>
-    <row r="22" spans="1:88">
+    <row r="22" spans="1:89">
       <c r="A22" s="1">
         <v>3430</v>
       </c>
@@ -6486,8 +6552,11 @@
       <c r="CJ22">
         <v>2</v>
       </c>
+      <c r="CK22">
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:88">
+    <row r="23" spans="1:89">
       <c r="A23" s="1">
         <v>3435</v>
       </c>
@@ -6752,8 +6821,11 @@
       <c r="CJ23">
         <v>0</v>
       </c>
+      <c r="CK23">
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:88">
+    <row r="24" spans="1:89">
       <c r="A24" s="1">
         <v>3560</v>
       </c>
@@ -7018,8 +7090,11 @@
       <c r="CJ24">
         <v>5</v>
       </c>
+      <c r="CK24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="25" spans="1:88">
+    <row r="25" spans="1:89">
       <c r="A25" s="1">
         <v>3578</v>
       </c>
@@ -7284,8 +7359,11 @@
       <c r="CJ25">
         <v>5</v>
       </c>
+      <c r="CK25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:88">
+    <row r="26" spans="1:89">
       <c r="A26" s="1">
         <v>3658</v>
       </c>
@@ -7550,8 +7628,11 @@
       <c r="CJ26">
         <v>5</v>
       </c>
+      <c r="CK26">
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:88">
+    <row r="27" spans="1:89">
       <c r="A27" s="1">
         <v>3771</v>
       </c>
@@ -7816,8 +7897,11 @@
       <c r="CJ27">
         <v>5</v>
       </c>
+      <c r="CK27">
+        <v>0</v>
+      </c>
     </row>
-    <row r="28" spans="1:88">
+    <row r="28" spans="1:89">
       <c r="A28" s="1">
         <v>4110</v>
       </c>
@@ -8082,8 +8166,11 @@
       <c r="CJ28">
         <v>5</v>
       </c>
+      <c r="CK28">
+        <v>0</v>
+      </c>
     </row>
-    <row r="29" spans="1:88">
+    <row r="29" spans="1:89">
       <c r="A29" s="1">
         <v>4178</v>
       </c>
@@ -8348,8 +8435,11 @@
       <c r="CJ29">
         <v>0</v>
       </c>
+      <c r="CK29">
+        <v>0</v>
+      </c>
     </row>
-    <row r="30" spans="1:88">
+    <row r="30" spans="1:89">
       <c r="A30" s="1">
         <v>4295</v>
       </c>
@@ -8614,8 +8704,11 @@
       <c r="CJ30">
         <v>5</v>
       </c>
+      <c r="CK30">
+        <v>0</v>
+      </c>
     </row>
-    <row r="31" spans="1:88">
+    <row r="31" spans="1:89">
       <c r="A31" s="1">
         <v>4415</v>
       </c>
@@ -8880,8 +8973,11 @@
       <c r="CJ31">
         <v>2</v>
       </c>
+      <c r="CK31">
+        <v>0</v>
+      </c>
     </row>
-    <row r="32" spans="1:88">
+    <row r="32" spans="1:89">
       <c r="A32" s="1">
         <v>4448</v>
       </c>
@@ -9146,8 +9242,11 @@
       <c r="CJ32">
         <v>5</v>
       </c>
+      <c r="CK32">
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:88">
+    <row r="33" spans="1:89">
       <c r="A33" s="1">
         <v>4785</v>
       </c>
@@ -9412,8 +9511,11 @@
       <c r="CJ33">
         <v>5</v>
       </c>
+      <c r="CK33">
+        <v>0</v>
+      </c>
     </row>
-    <row r="34" spans="1:88">
+    <row r="34" spans="1:89">
       <c r="A34" s="1">
         <v>4943</v>
       </c>
@@ -9678,8 +9780,11 @@
       <c r="CJ34">
         <v>5</v>
       </c>
+      <c r="CK34">
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="1:88">
+    <row r="35" spans="1:89">
       <c r="A35" s="1">
         <v>5213</v>
       </c>
@@ -9944,8 +10049,11 @@
       <c r="CJ35">
         <v>5</v>
       </c>
+      <c r="CK35">
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:88">
+    <row r="36" spans="1:89">
       <c r="A36" s="1">
         <v>5259</v>
       </c>
@@ -10210,8 +10318,11 @@
       <c r="CJ36">
         <v>5</v>
       </c>
+      <c r="CK36">
+        <v>0</v>
+      </c>
     </row>
-    <row r="37" spans="1:88">
+    <row r="37" spans="1:89">
       <c r="A37" s="1">
         <v>5421</v>
       </c>
@@ -10476,8 +10587,11 @@
       <c r="CJ37">
         <v>2</v>
       </c>
+      <c r="CK37">
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="1:88">
+    <row r="38" spans="1:89">
       <c r="A38" s="1">
         <v>5546</v>
       </c>
@@ -10742,8 +10856,11 @@
       <c r="CJ38">
         <v>5</v>
       </c>
+      <c r="CK38">
+        <v>0</v>
+      </c>
     </row>
-    <row r="39" spans="1:88">
+    <row r="39" spans="1:89">
       <c r="A39" s="1">
         <v>5665</v>
       </c>
@@ -11008,8 +11125,11 @@
       <c r="CJ39">
         <v>0</v>
       </c>
+      <c r="CK39">
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:88">
+    <row r="40" spans="1:89">
       <c r="A40" s="1">
         <v>5739</v>
       </c>
@@ -11274,8 +11394,11 @@
       <c r="CJ40">
         <v>2</v>
       </c>
+      <c r="CK40">
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:88">
+    <row r="41" spans="1:89">
       <c r="A41" s="1">
         <v>5769</v>
       </c>
@@ -11540,8 +11663,11 @@
       <c r="CJ41">
         <v>0</v>
       </c>
+      <c r="CK41">
+        <v>0</v>
+      </c>
     </row>
-    <row r="42" spans="1:88">
+    <row r="42" spans="1:89">
       <c r="A42" s="1">
         <v>5814</v>
       </c>
@@ -11806,8 +11932,11 @@
       <c r="CJ42">
         <v>5</v>
       </c>
+      <c r="CK42">
+        <v>0</v>
+      </c>
     </row>
-    <row r="43" spans="1:88">
+    <row r="43" spans="1:89">
       <c r="A43" s="1">
         <v>5816</v>
       </c>
@@ -12072,8 +12201,11 @@
       <c r="CJ43">
         <v>6</v>
       </c>
+      <c r="CK43">
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:88">
+    <row r="44" spans="1:89">
       <c r="A44" s="1">
         <v>5875</v>
       </c>
@@ -12338,8 +12470,11 @@
       <c r="CJ44">
         <v>0</v>
       </c>
+      <c r="CK44">
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:88">
+    <row r="45" spans="1:89">
       <c r="A45" s="1">
         <v>5881</v>
       </c>
@@ -12604,8 +12739,11 @@
       <c r="CJ45">
         <v>5</v>
       </c>
+      <c r="CK45">
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:88">
+    <row r="46" spans="1:89">
       <c r="A46" s="1">
         <v>5897</v>
       </c>
@@ -12870,8 +13008,11 @@
       <c r="CJ46">
         <v>5</v>
       </c>
+      <c r="CK46">
+        <v>0</v>
+      </c>
     </row>
-    <row r="47" spans="1:88">
+    <row r="47" spans="1:89">
       <c r="A47" s="1">
         <v>5961</v>
       </c>
@@ -13136,8 +13277,11 @@
       <c r="CJ47">
         <v>1</v>
       </c>
+      <c r="CK47">
+        <v>0</v>
+      </c>
     </row>
-    <row r="48" spans="1:88">
+    <row r="48" spans="1:89">
       <c r="A48" s="1">
         <v>6159</v>
       </c>
@@ -13402,8 +13546,11 @@
       <c r="CJ48">
         <v>0</v>
       </c>
+      <c r="CK48">
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:88">
+    <row r="49" spans="1:89">
       <c r="A49" s="1">
         <v>6336</v>
       </c>
@@ -13668,8 +13815,11 @@
       <c r="CJ49">
         <v>6</v>
       </c>
+      <c r="CK49">
+        <v>0</v>
+      </c>
     </row>
-    <row r="50" spans="1:88">
+    <row r="50" spans="1:89">
       <c r="A50" s="1">
         <v>6365</v>
       </c>
@@ -13934,8 +14084,11 @@
       <c r="CJ50">
         <v>0</v>
       </c>
+      <c r="CK50">
+        <v>0</v>
+      </c>
     </row>
-    <row r="51" spans="1:88">
+    <row r="51" spans="1:89">
       <c r="A51" s="1">
         <v>6368</v>
       </c>
@@ -14200,8 +14353,11 @@
       <c r="CJ51">
         <v>6</v>
       </c>
+      <c r="CK51">
+        <v>0</v>
+      </c>
     </row>
-    <row r="52" spans="1:88">
+    <row r="52" spans="1:89">
       <c r="A52" s="1">
         <v>6409</v>
       </c>
@@ -14466,8 +14622,11 @@
       <c r="CJ52">
         <v>5</v>
       </c>
+      <c r="CK52">
+        <v>0</v>
+      </c>
     </row>
-    <row r="53" spans="1:88">
+    <row r="53" spans="1:89">
       <c r="A53" s="1">
         <v>6428</v>
       </c>
@@ -14732,8 +14891,11 @@
       <c r="CJ53">
         <v>5</v>
       </c>
+      <c r="CK53">
+        <v>0</v>
+      </c>
     </row>
-    <row r="54" spans="1:88">
+    <row r="54" spans="1:89">
       <c r="A54" s="1">
         <v>6451</v>
       </c>
@@ -14998,8 +15160,11 @@
       <c r="CJ54">
         <v>10</v>
       </c>
+      <c r="CK54">
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:88">
+    <row r="55" spans="1:89">
       <c r="A55" s="1">
         <v>6459</v>
       </c>
@@ -15264,8 +15429,11 @@
       <c r="CJ55">
         <v>0</v>
       </c>
+      <c r="CK55">
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:88">
+    <row r="56" spans="1:89">
       <c r="A56" s="1">
         <v>6481</v>
       </c>
@@ -15530,8 +15698,11 @@
       <c r="CJ56">
         <v>5</v>
       </c>
+      <c r="CK56">
+        <v>0</v>
+      </c>
     </row>
-    <row r="57" spans="1:88">
+    <row r="57" spans="1:89">
       <c r="A57" s="1">
         <v>6487</v>
       </c>
@@ -15796,8 +15967,11 @@
       <c r="CJ57">
         <v>5</v>
       </c>
+      <c r="CK57">
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:88">
+    <row r="58" spans="1:89">
       <c r="A58" s="1">
         <v>6506</v>
       </c>
@@ -16062,8 +16236,11 @@
       <c r="CJ58">
         <v>5</v>
       </c>
+      <c r="CK58">
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:88">
+    <row r="59" spans="1:89">
       <c r="A59" s="1">
         <v>6648</v>
       </c>
@@ -16328,8 +16505,11 @@
       <c r="CJ59">
         <v>5</v>
       </c>
+      <c r="CK59">
+        <v>0</v>
+      </c>
     </row>
-    <row r="60" spans="1:88">
+    <row r="60" spans="1:89">
       <c r="A60" s="1">
         <v>6726</v>
       </c>
@@ -16594,8 +16774,11 @@
       <c r="CJ60">
         <v>0</v>
       </c>
+      <c r="CK60">
+        <v>0</v>
+      </c>
     </row>
-    <row r="61" spans="1:88">
+    <row r="61" spans="1:89">
       <c r="A61" s="1">
         <v>6810</v>
       </c>
@@ -16860,8 +17043,11 @@
       <c r="CJ61">
         <v>3</v>
       </c>
+      <c r="CK61">
+        <v>0</v>
+      </c>
     </row>
-    <row r="62" spans="1:88">
+    <row r="62" spans="1:89">
       <c r="A62" s="1">
         <v>6891</v>
       </c>
@@ -17126,8 +17312,11 @@
       <c r="CJ62">
         <v>0</v>
       </c>
+      <c r="CK62">
+        <v>0</v>
+      </c>
     </row>
-    <row r="63" spans="1:88">
+    <row r="63" spans="1:89">
       <c r="A63" s="1">
         <v>6935</v>
       </c>
@@ -17392,8 +17581,11 @@
       <c r="CJ63">
         <v>0</v>
       </c>
+      <c r="CK63">
+        <v>0</v>
+      </c>
     </row>
-    <row r="64" spans="1:88">
+    <row r="64" spans="1:89">
       <c r="A64" s="1">
         <v>6940</v>
       </c>
@@ -17658,8 +17850,11 @@
       <c r="CJ64">
         <v>0</v>
       </c>
+      <c r="CK64">
+        <v>0</v>
+      </c>
     </row>
-    <row r="65" spans="1:88">
+    <row r="65" spans="1:89">
       <c r="A65" s="1">
         <v>7029</v>
       </c>
@@ -17924,8 +18119,11 @@
       <c r="CJ65">
         <v>6</v>
       </c>
+      <c r="CK65">
+        <v>0</v>
+      </c>
     </row>
-    <row r="66" spans="1:88">
+    <row r="66" spans="1:89">
       <c r="A66" s="1">
         <v>7049</v>
       </c>
@@ -18190,8 +18388,11 @@
       <c r="CJ66">
         <v>6</v>
       </c>
+      <c r="CK66">
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:88">
+    <row r="67" spans="1:89">
       <c r="A67" s="1">
         <v>7137</v>
       </c>
@@ -18456,8 +18657,11 @@
       <c r="CJ67">
         <v>5</v>
       </c>
+      <c r="CK67">
+        <v>0</v>
+      </c>
     </row>
-    <row r="68" spans="1:88">
+    <row r="68" spans="1:89">
       <c r="A68" s="1">
         <v>7140</v>
       </c>
@@ -18722,8 +18926,11 @@
       <c r="CJ68">
         <v>2</v>
       </c>
+      <c r="CK68">
+        <v>0</v>
+      </c>
     </row>
-    <row r="69" spans="1:88">
+    <row r="69" spans="1:89">
       <c r="A69" s="1">
         <v>7162</v>
       </c>
@@ -18988,8 +19195,11 @@
       <c r="CJ69">
         <v>5</v>
       </c>
+      <c r="CK69">
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:88">
+    <row r="70" spans="1:89">
       <c r="A70" s="1">
         <v>7224</v>
       </c>
@@ -19254,8 +19464,11 @@
       <c r="CJ70">
         <v>0</v>
       </c>
+      <c r="CK70">
+        <v>0</v>
+      </c>
     </row>
-    <row r="71" spans="1:88">
+    <row r="71" spans="1:89">
       <c r="A71" s="1">
         <v>7313</v>
       </c>
@@ -19520,8 +19733,11 @@
       <c r="CJ71">
         <v>5</v>
       </c>
+      <c r="CK71">
+        <v>0</v>
+      </c>
     </row>
-    <row r="72" spans="1:88">
+    <row r="72" spans="1:89">
       <c r="A72" s="1">
         <v>7319</v>
       </c>
@@ -19786,8 +20002,11 @@
       <c r="CJ72">
         <v>5</v>
       </c>
+      <c r="CK72">
+        <v>0</v>
+      </c>
     </row>
-    <row r="73" spans="1:88">
+    <row r="73" spans="1:89">
       <c r="A73" s="1">
         <v>7399</v>
       </c>
@@ -20052,8 +20271,11 @@
       <c r="CJ73">
         <v>0</v>
       </c>
+      <c r="CK73">
+        <v>0</v>
+      </c>
     </row>
-    <row r="74" spans="1:88">
+    <row r="74" spans="1:89">
       <c r="A74" s="1">
         <v>7471</v>
       </c>
@@ -20318,8 +20540,11 @@
       <c r="CJ74">
         <v>2</v>
       </c>
+      <c r="CK74">
+        <v>0</v>
+      </c>
     </row>
-    <row r="75" spans="1:88">
+    <row r="75" spans="1:89">
       <c r="A75" s="1">
         <v>7482</v>
       </c>
@@ -20584,8 +20809,11 @@
       <c r="CJ75">
         <v>5</v>
       </c>
+      <c r="CK75">
+        <v>0</v>
+      </c>
     </row>
-    <row r="76" spans="1:88">
+    <row r="76" spans="1:89">
       <c r="A76" s="1">
         <v>7560</v>
       </c>
@@ -20850,8 +21078,11 @@
       <c r="CJ76">
         <v>5</v>
       </c>
+      <c r="CK76">
+        <v>0</v>
+      </c>
     </row>
-    <row r="77" spans="1:88">
+    <row r="77" spans="1:89">
       <c r="A77" s="1">
         <v>7577</v>
       </c>
@@ -21116,8 +21347,11 @@
       <c r="CJ77">
         <v>5</v>
       </c>
+      <c r="CK77">
+        <v>0</v>
+      </c>
     </row>
-    <row r="78" spans="1:88">
+    <row r="78" spans="1:89">
       <c r="A78" s="1">
         <v>7615</v>
       </c>
@@ -21382,8 +21616,11 @@
       <c r="CJ78">
         <v>2</v>
       </c>
+      <c r="CK78">
+        <v>0</v>
+      </c>
     </row>
-    <row r="79" spans="1:88">
+    <row r="79" spans="1:89">
       <c r="A79" s="1">
         <v>7648</v>
       </c>
@@ -21648,8 +21885,11 @@
       <c r="CJ79">
         <v>0</v>
       </c>
+      <c r="CK79">
+        <v>0</v>
+      </c>
     </row>
-    <row r="80" spans="1:88">
+    <row r="80" spans="1:89">
       <c r="A80" s="1">
         <v>7688</v>
       </c>
@@ -21914,8 +22154,11 @@
       <c r="CJ80">
         <v>0</v>
       </c>
+      <c r="CK80">
+        <v>0</v>
+      </c>
     </row>
-    <row r="81" spans="1:88">
+    <row r="81" spans="1:89">
       <c r="A81" s="1">
         <v>7696</v>
       </c>
@@ -22180,8 +22423,11 @@
       <c r="CJ81">
         <v>3</v>
       </c>
+      <c r="CK81">
+        <v>0</v>
+      </c>
     </row>
-    <row r="82" spans="1:88">
+    <row r="82" spans="1:89">
       <c r="A82" s="1">
         <v>7722</v>
       </c>
@@ -22446,8 +22692,11 @@
       <c r="CJ82">
         <v>5</v>
       </c>
+      <c r="CK82">
+        <v>0</v>
+      </c>
     </row>
-    <row r="83" spans="1:88">
+    <row r="83" spans="1:89">
       <c r="A83" s="1">
         <v>7778</v>
       </c>
@@ -22712,8 +22961,11 @@
       <c r="CJ83">
         <v>0</v>
       </c>
+      <c r="CK83">
+        <v>0</v>
+      </c>
     </row>
-    <row r="84" spans="1:88">
+    <row r="84" spans="1:89">
       <c r="A84" s="1">
         <v>7814</v>
       </c>
@@ -22978,8 +23230,11 @@
       <c r="CJ84">
         <v>0</v>
       </c>
+      <c r="CK84">
+        <v>0</v>
+      </c>
     </row>
-    <row r="85" spans="1:88">
+    <row r="85" spans="1:89">
       <c r="A85" s="1">
         <v>7850</v>
       </c>
@@ -23244,8 +23499,11 @@
       <c r="CJ85">
         <v>2</v>
       </c>
+      <c r="CK85">
+        <v>0</v>
+      </c>
     </row>
-    <row r="86" spans="1:88">
+    <row r="86" spans="1:89">
       <c r="A86" s="1">
         <v>7924</v>
       </c>
@@ -23510,8 +23768,11 @@
       <c r="CJ86">
         <v>0</v>
       </c>
+      <c r="CK86">
+        <v>0</v>
+      </c>
     </row>
-    <row r="87" spans="1:88">
+    <row r="87" spans="1:89">
       <c r="A87" s="1">
         <v>7985</v>
       </c>
@@ -23776,8 +24037,11 @@
       <c r="CJ87">
         <v>5</v>
       </c>
+      <c r="CK87">
+        <v>0</v>
+      </c>
     </row>
-    <row r="88" spans="1:88">
+    <row r="88" spans="1:89">
       <c r="A88" s="1">
         <v>8026</v>
       </c>
@@ -24042,8 +24306,11 @@
       <c r="CJ88">
         <v>5</v>
       </c>
+      <c r="CK88">
+        <v>0</v>
+      </c>
     </row>
-    <row r="89" spans="1:88">
+    <row r="89" spans="1:89">
       <c r="A89" s="1">
         <v>8028</v>
       </c>
@@ -24308,8 +24575,11 @@
       <c r="CJ89">
         <v>0</v>
       </c>
+      <c r="CK89">
+        <v>0</v>
+      </c>
     </row>
-    <row r="90" spans="1:88">
+    <row r="90" spans="1:89">
       <c r="A90" s="1">
         <v>8036</v>
       </c>
@@ -24574,8 +24844,11 @@
       <c r="CJ90">
         <v>3</v>
       </c>
+      <c r="CK90">
+        <v>0</v>
+      </c>
     </row>
-    <row r="91" spans="1:88">
+    <row r="91" spans="1:89">
       <c r="A91" s="1">
         <v>8108</v>
       </c>
@@ -24840,8 +25113,11 @@
       <c r="CJ91">
         <v>5</v>
       </c>
+      <c r="CK91">
+        <v>0</v>
+      </c>
     </row>
-    <row r="92" spans="1:88">
+    <row r="92" spans="1:89">
       <c r="A92" s="1">
         <v>8164</v>
       </c>
@@ -25106,8 +25382,11 @@
       <c r="CJ92">
         <v>0</v>
       </c>
+      <c r="CK92">
+        <v>0</v>
+      </c>
     </row>
-    <row r="93" spans="1:88">
+    <row r="93" spans="1:89">
       <c r="A93" s="1">
         <v>8242</v>
       </c>
@@ -25372,8 +25651,11 @@
       <c r="CJ93">
         <v>0</v>
       </c>
+      <c r="CK93">
+        <v>0</v>
+      </c>
     </row>
-    <row r="94" spans="1:88">
+    <row r="94" spans="1:89">
       <c r="A94" s="1">
         <v>8345</v>
       </c>
@@ -25638,8 +25920,11 @@
       <c r="CJ94">
         <v>6</v>
       </c>
+      <c r="CK94">
+        <v>0</v>
+      </c>
     </row>
-    <row r="95" spans="1:88">
+    <row r="95" spans="1:89">
       <c r="A95" s="1">
         <v>8400</v>
       </c>
@@ -25904,8 +26189,11 @@
       <c r="CJ95">
         <v>1</v>
       </c>
+      <c r="CK95">
+        <v>0</v>
+      </c>
     </row>
-    <row r="96" spans="1:88">
+    <row r="96" spans="1:89">
       <c r="A96" s="1">
         <v>8462</v>
       </c>
@@ -26170,8 +26458,11 @@
       <c r="CJ96">
         <v>6</v>
       </c>
+      <c r="CK96">
+        <v>0</v>
+      </c>
     </row>
-    <row r="97" spans="1:88">
+    <row r="97" spans="1:89">
       <c r="A97" s="1">
         <v>8478</v>
       </c>
@@ -26436,8 +26727,11 @@
       <c r="CJ97">
         <v>2</v>
       </c>
+      <c r="CK97">
+        <v>0</v>
+      </c>
     </row>
-    <row r="98" spans="1:88">
+    <row r="98" spans="1:89">
       <c r="A98" s="1">
         <v>8503</v>
       </c>
@@ -26702,8 +26996,11 @@
       <c r="CJ98">
         <v>5</v>
       </c>
+      <c r="CK98">
+        <v>0</v>
+      </c>
     </row>
-    <row r="99" spans="1:88">
+    <row r="99" spans="1:89">
       <c r="A99" s="1">
         <v>8521</v>
       </c>
@@ -26968,8 +27265,11 @@
       <c r="CJ99">
         <v>5</v>
       </c>
+      <c r="CK99">
+        <v>0</v>
+      </c>
     </row>
-    <row r="100" spans="1:88">
+    <row r="100" spans="1:89">
       <c r="A100" s="1">
         <v>8537</v>
       </c>
@@ -27234,8 +27534,11 @@
       <c r="CJ100">
         <v>0</v>
       </c>
+      <c r="CK100">
+        <v>0</v>
+      </c>
     </row>
-    <row r="101" spans="1:88">
+    <row r="101" spans="1:89">
       <c r="A101" s="1">
         <v>8568</v>
       </c>
@@ -27500,8 +27803,11 @@
       <c r="CJ101">
         <v>5</v>
       </c>
+      <c r="CK101">
+        <v>0</v>
+      </c>
     </row>
-    <row r="102" spans="1:88">
+    <row r="102" spans="1:89">
       <c r="A102" s="1">
         <v>8616</v>
       </c>
@@ -27766,8 +28072,11 @@
       <c r="CJ102">
         <v>1</v>
       </c>
+      <c r="CK102">
+        <v>0</v>
+      </c>
     </row>
-    <row r="103" spans="1:88">
+    <row r="103" spans="1:89">
       <c r="A103" s="1">
         <v>8682</v>
       </c>
@@ -28032,8 +28341,11 @@
       <c r="CJ103">
         <v>0</v>
       </c>
+      <c r="CK103">
+        <v>0</v>
+      </c>
     </row>
-    <row r="104" spans="1:88">
+    <row r="104" spans="1:89">
       <c r="A104" s="1">
         <v>8714</v>
       </c>
@@ -28298,8 +28610,11 @@
       <c r="CJ104">
         <v>5</v>
       </c>
+      <c r="CK104">
+        <v>0</v>
+      </c>
     </row>
-    <row r="105" spans="1:88">
+    <row r="105" spans="1:89">
       <c r="A105" s="1">
         <v>8735</v>
       </c>
@@ -28564,8 +28879,11 @@
       <c r="CJ105">
         <v>6</v>
       </c>
+      <c r="CK105">
+        <v>0</v>
+      </c>
     </row>
-    <row r="106" spans="1:88">
+    <row r="106" spans="1:89">
       <c r="A106" s="1">
         <v>8758</v>
       </c>
@@ -28830,8 +29148,11 @@
       <c r="CJ106">
         <v>4</v>
       </c>
+      <c r="CK106">
+        <v>0</v>
+      </c>
     </row>
-    <row r="107" spans="1:88">
+    <row r="107" spans="1:89">
       <c r="A107" s="1">
         <v>8789</v>
       </c>
@@ -29096,8 +29417,11 @@
       <c r="CJ107">
         <v>2</v>
       </c>
+      <c r="CK107">
+        <v>0</v>
+      </c>
     </row>
-    <row r="108" spans="1:88">
+    <row r="108" spans="1:89">
       <c r="A108" s="1">
         <v>8792</v>
       </c>
@@ -29362,8 +29686,11 @@
       <c r="CJ108">
         <v>5</v>
       </c>
+      <c r="CK108">
+        <v>0</v>
+      </c>
     </row>
-    <row r="109" spans="1:88">
+    <row r="109" spans="1:89">
       <c r="A109" s="1">
         <v>8805</v>
       </c>
@@ -29628,8 +29955,11 @@
       <c r="CJ109">
         <v>2</v>
       </c>
+      <c r="CK109">
+        <v>0</v>
+      </c>
     </row>
-    <row r="110" spans="1:88">
+    <row r="110" spans="1:89">
       <c r="A110" s="1">
         <v>8889</v>
       </c>
@@ -29894,8 +30224,11 @@
       <c r="CJ110">
         <v>5</v>
       </c>
+      <c r="CK110">
+        <v>0</v>
+      </c>
     </row>
-    <row r="111" spans="1:88">
+    <row r="111" spans="1:89">
       <c r="A111" s="1">
         <v>8959</v>
       </c>
@@ -30160,8 +30493,11 @@
       <c r="CJ111">
         <v>6</v>
       </c>
+      <c r="CK111">
+        <v>0</v>
+      </c>
     </row>
-    <row r="112" spans="1:88">
+    <row r="112" spans="1:89">
       <c r="A112" s="1">
         <v>8966</v>
       </c>
@@ -30426,8 +30762,11 @@
       <c r="CJ112">
         <v>2</v>
       </c>
+      <c r="CK112">
+        <v>0</v>
+      </c>
     </row>
-    <row r="113" spans="1:88">
+    <row r="113" spans="1:89">
       <c r="A113" s="1">
         <v>9018</v>
       </c>
@@ -30692,8 +31031,11 @@
       <c r="CJ113">
         <v>0</v>
       </c>
+      <c r="CK113">
+        <v>0</v>
+      </c>
     </row>
-    <row r="114" spans="1:88">
+    <row r="114" spans="1:89">
       <c r="A114" s="1">
         <v>9032</v>
       </c>
@@ -30958,8 +31300,11 @@
       <c r="CJ114">
         <v>10</v>
       </c>
+      <c r="CK114">
+        <v>0</v>
+      </c>
     </row>
-    <row r="115" spans="1:88">
+    <row r="115" spans="1:89">
       <c r="A115" s="1">
         <v>9054</v>
       </c>
@@ -31224,8 +31569,11 @@
       <c r="CJ115">
         <v>0</v>
       </c>
+      <c r="CK115">
+        <v>0</v>
+      </c>
     </row>
-    <row r="116" spans="1:88">
+    <row r="116" spans="1:89">
       <c r="A116" s="1">
         <v>9103</v>
       </c>
@@ -31490,8 +31838,11 @@
       <c r="CJ116">
         <v>0</v>
       </c>
+      <c r="CK116">
+        <v>0</v>
+      </c>
     </row>
-    <row r="117" spans="1:88">
+    <row r="117" spans="1:89">
       <c r="A117" s="1">
         <v>9146</v>
       </c>
@@ -31756,8 +32107,11 @@
       <c r="CJ117">
         <v>0</v>
       </c>
+      <c r="CK117">
+        <v>0</v>
+      </c>
     </row>
-    <row r="118" spans="1:88">
+    <row r="118" spans="1:89">
       <c r="A118" s="1">
         <v>9251</v>
       </c>
@@ -32022,8 +32376,11 @@
       <c r="CJ118">
         <v>4</v>
       </c>
+      <c r="CK118">
+        <v>0</v>
+      </c>
     </row>
-    <row r="119" spans="1:88">
+    <row r="119" spans="1:89">
       <c r="A119" s="1">
         <v>9263</v>
       </c>
@@ -32288,8 +32645,11 @@
       <c r="CJ119">
         <v>5</v>
       </c>
+      <c r="CK119">
+        <v>0</v>
+      </c>
     </row>
-    <row r="120" spans="1:88">
+    <row r="120" spans="1:89">
       <c r="A120" s="1">
         <v>9346</v>
       </c>
@@ -32554,8 +32914,11 @@
       <c r="CJ120">
         <v>0</v>
       </c>
+      <c r="CK120">
+        <v>0</v>
+      </c>
     </row>
-    <row r="121" spans="1:88">
+    <row r="121" spans="1:89">
       <c r="A121" s="1">
         <v>9359</v>
       </c>
@@ -32820,8 +33183,11 @@
       <c r="CJ121">
         <v>5</v>
       </c>
+      <c r="CK121">
+        <v>0</v>
+      </c>
     </row>
-    <row r="122" spans="1:88">
+    <row r="122" spans="1:89">
       <c r="A122" s="1">
         <v>9373</v>
       </c>
@@ -33086,8 +33452,11 @@
       <c r="CJ122">
         <v>5</v>
       </c>
+      <c r="CK122">
+        <v>0</v>
+      </c>
     </row>
-    <row r="123" spans="1:88">
+    <row r="123" spans="1:89">
       <c r="A123" s="1">
         <v>9414</v>
       </c>
@@ -33352,8 +33721,11 @@
       <c r="CJ123">
         <v>5</v>
       </c>
+      <c r="CK123">
+        <v>0</v>
+      </c>
     </row>
-    <row r="124" spans="1:88">
+    <row r="124" spans="1:89">
       <c r="A124" s="1">
         <v>9435</v>
       </c>
@@ -33618,8 +33990,11 @@
       <c r="CJ124">
         <v>6</v>
       </c>
+      <c r="CK124">
+        <v>0</v>
+      </c>
     </row>
-    <row r="125" spans="1:88">
+    <row r="125" spans="1:89">
       <c r="A125" s="1">
         <v>9492</v>
       </c>
@@ -33884,8 +34259,11 @@
       <c r="CJ125">
         <v>1</v>
       </c>
+      <c r="CK125">
+        <v>0</v>
+      </c>
     </row>
-    <row r="126" spans="1:88">
+    <row r="126" spans="1:89">
       <c r="A126" s="1">
         <v>9501</v>
       </c>
@@ -34150,8 +34528,11 @@
       <c r="CJ126">
         <v>0</v>
       </c>
+      <c r="CK126">
+        <v>0</v>
+      </c>
     </row>
-    <row r="127" spans="1:88">
+    <row r="127" spans="1:89">
       <c r="A127" s="1">
         <v>9553</v>
       </c>
@@ -34416,8 +34797,11 @@
       <c r="CJ127">
         <v>2</v>
       </c>
+      <c r="CK127">
+        <v>0</v>
+      </c>
     </row>
-    <row r="128" spans="1:88">
+    <row r="128" spans="1:89">
       <c r="A128" s="1">
         <v>9558</v>
       </c>
@@ -34682,8 +35066,11 @@
       <c r="CJ128">
         <v>4</v>
       </c>
+      <c r="CK128">
+        <v>0</v>
+      </c>
     </row>
-    <row r="129" spans="1:88">
+    <row r="129" spans="1:89">
       <c r="A129" s="1">
         <v>9567</v>
       </c>
@@ -34948,8 +35335,11 @@
       <c r="CJ129">
         <v>4</v>
       </c>
+      <c r="CK129">
+        <v>0</v>
+      </c>
     </row>
-    <row r="130" spans="1:88">
+    <row r="130" spans="1:89">
       <c r="A130" s="1">
         <v>9660</v>
       </c>
@@ -35214,8 +35604,11 @@
       <c r="CJ130">
         <v>5</v>
       </c>
+      <c r="CK130">
+        <v>0</v>
+      </c>
     </row>
-    <row r="131" spans="1:88">
+    <row r="131" spans="1:89">
       <c r="A131" s="1">
         <v>9670</v>
       </c>
@@ -35480,8 +35873,11 @@
       <c r="CJ131">
         <v>5</v>
       </c>
+      <c r="CK131">
+        <v>0</v>
+      </c>
     </row>
-    <row r="132" spans="1:88">
+    <row r="132" spans="1:89">
       <c r="A132" s="1">
         <v>9690</v>
       </c>
@@ -35746,8 +36142,11 @@
       <c r="CJ132">
         <v>0</v>
       </c>
+      <c r="CK132">
+        <v>0</v>
+      </c>
     </row>
-    <row r="133" spans="1:88">
+    <row r="133" spans="1:89">
       <c r="A133" s="1">
         <v>9772</v>
       </c>
@@ -36012,8 +36411,11 @@
       <c r="CJ133">
         <v>5</v>
       </c>
+      <c r="CK133">
+        <v>0</v>
+      </c>
     </row>
-    <row r="134" spans="1:88">
+    <row r="134" spans="1:89">
       <c r="A134" s="1">
         <v>9902</v>
       </c>
@@ -36278,8 +36680,11 @@
       <c r="CJ134">
         <v>5</v>
       </c>
+      <c r="CK134">
+        <v>0</v>
+      </c>
     </row>
-    <row r="135" spans="1:88">
+    <row r="135" spans="1:89">
       <c r="A135" s="1">
         <v>9949</v>
       </c>
@@ -36544,8 +36949,11 @@
       <c r="CJ135">
         <v>5</v>
       </c>
+      <c r="CK135">
+        <v>0</v>
+      </c>
     </row>
-    <row r="136" spans="1:88">
+    <row r="136" spans="1:89">
       <c r="A136" s="1">
         <v>9968</v>
       </c>
@@ -36810,8 +37218,11 @@
       <c r="CJ136">
         <v>5</v>
       </c>
+      <c r="CK136">
+        <v>0</v>
+      </c>
     </row>
-    <row r="137" spans="1:88">
+    <row r="137" spans="1:89">
       <c r="A137" s="1">
         <v>9972</v>
       </c>
@@ -37076,8 +37487,11 @@
       <c r="CJ137">
         <v>4</v>
       </c>
+      <c r="CK137">
+        <v>0</v>
+      </c>
     </row>
-    <row r="138" spans="1:88">
+    <row r="138" spans="1:89">
       <c r="A138" s="1">
         <v>10124</v>
       </c>
@@ -37342,8 +37756,11 @@
       <c r="CJ138">
         <v>5</v>
       </c>
+      <c r="CK138">
+        <v>0</v>
+      </c>
     </row>
-    <row r="139" spans="1:88">
+    <row r="139" spans="1:89">
       <c r="A139" s="1">
         <v>10144</v>
       </c>
@@ -37608,8 +38025,11 @@
       <c r="CJ139">
         <v>1</v>
       </c>
+      <c r="CK139">
+        <v>0</v>
+      </c>
     </row>
-    <row r="140" spans="1:88">
+    <row r="140" spans="1:89">
       <c r="A140" s="1">
         <v>10190</v>
       </c>
@@ -37874,8 +38294,11 @@
       <c r="CJ140">
         <v>0</v>
       </c>
+      <c r="CK140">
+        <v>0</v>
+      </c>
     </row>
-    <row r="141" spans="1:88">
+    <row r="141" spans="1:89">
       <c r="A141" s="1">
         <v>10243</v>
       </c>
@@ -38140,8 +38563,11 @@
       <c r="CJ141">
         <v>0</v>
       </c>
+      <c r="CK141">
+        <v>0</v>
+      </c>
     </row>
-    <row r="142" spans="1:88">
+    <row r="142" spans="1:89">
       <c r="A142" s="1">
         <v>10269</v>
       </c>
@@ -38406,8 +38832,11 @@
       <c r="CJ142">
         <v>5</v>
       </c>
+      <c r="CK142">
+        <v>0</v>
+      </c>
     </row>
-    <row r="143" spans="1:88">
+    <row r="143" spans="1:89">
       <c r="A143" s="1">
         <v>10298</v>
       </c>
@@ -38672,8 +39101,11 @@
       <c r="CJ143">
         <v>5</v>
       </c>
+      <c r="CK143">
+        <v>0</v>
+      </c>
     </row>
-    <row r="144" spans="1:88">
+    <row r="144" spans="1:89">
       <c r="A144" s="1">
         <v>10332</v>
       </c>
@@ -38938,8 +39370,11 @@
       <c r="CJ144">
         <v>2</v>
       </c>
+      <c r="CK144">
+        <v>0</v>
+      </c>
     </row>
-    <row r="145" spans="1:88">
+    <row r="145" spans="1:89">
       <c r="A145" s="1">
         <v>10361</v>
       </c>
@@ -39204,8 +39639,11 @@
       <c r="CJ145">
         <v>2</v>
       </c>
+      <c r="CK145">
+        <v>0</v>
+      </c>
     </row>
-    <row r="146" spans="1:88">
+    <row r="146" spans="1:89">
       <c r="A146" s="1">
         <v>10362</v>
       </c>
@@ -39470,8 +39908,11 @@
       <c r="CJ146">
         <v>0</v>
       </c>
+      <c r="CK146">
+        <v>0</v>
+      </c>
     </row>
-    <row r="147" spans="1:88">
+    <row r="147" spans="1:89">
       <c r="A147" s="1">
         <v>10398</v>
       </c>
@@ -39736,8 +40177,11 @@
       <c r="CJ147">
         <v>0</v>
       </c>
+      <c r="CK147">
+        <v>0</v>
+      </c>
     </row>
-    <row r="148" spans="1:88">
+    <row r="148" spans="1:89">
       <c r="A148" s="1">
         <v>10404</v>
       </c>
@@ -40002,8 +40446,11 @@
       <c r="CJ148">
         <v>0</v>
       </c>
+      <c r="CK148">
+        <v>0</v>
+      </c>
     </row>
-    <row r="149" spans="1:88">
+    <row r="149" spans="1:89">
       <c r="A149" s="1">
         <v>10427</v>
       </c>
@@ -40268,8 +40715,11 @@
       <c r="CJ149">
         <v>0</v>
       </c>
+      <c r="CK149">
+        <v>0</v>
+      </c>
     </row>
-    <row r="150" spans="1:88">
+    <row r="150" spans="1:89">
       <c r="A150" s="1">
         <v>10440</v>
       </c>
@@ -40534,8 +40984,11 @@
       <c r="CJ150">
         <v>5</v>
       </c>
+      <c r="CK150">
+        <v>0</v>
+      </c>
     </row>
-    <row r="151" spans="1:88">
+    <row r="151" spans="1:89">
       <c r="A151" s="1">
         <v>10454</v>
       </c>
@@ -40800,8 +41253,11 @@
       <c r="CJ151">
         <v>2</v>
       </c>
+      <c r="CK151">
+        <v>0</v>
+      </c>
     </row>
-    <row r="152" spans="1:88">
+    <row r="152" spans="1:89">
       <c r="A152" s="1">
         <v>10469</v>
       </c>
@@ -41066,8 +41522,11 @@
       <c r="CJ152">
         <v>5</v>
       </c>
+      <c r="CK152">
+        <v>0</v>
+      </c>
     </row>
-    <row r="153" spans="1:88">
+    <row r="153" spans="1:89">
       <c r="A153" s="1">
         <v>10562</v>
       </c>
@@ -41332,8 +41791,11 @@
       <c r="CJ153">
         <v>0</v>
       </c>
+      <c r="CK153">
+        <v>0</v>
+      </c>
     </row>
-    <row r="154" spans="1:88">
+    <row r="154" spans="1:89">
       <c r="A154" s="1">
         <v>10576</v>
       </c>
@@ -41598,8 +42060,11 @@
       <c r="CJ154">
         <v>0</v>
       </c>
+      <c r="CK154">
+        <v>0</v>
+      </c>
     </row>
-    <row r="155" spans="1:88">
+    <row r="155" spans="1:89">
       <c r="A155" s="1">
         <v>10609</v>
       </c>
@@ -41864,8 +42329,11 @@
       <c r="CJ155">
         <v>2</v>
       </c>
+      <c r="CK155">
+        <v>0</v>
+      </c>
     </row>
-    <row r="156" spans="1:88">
+    <row r="156" spans="1:89">
       <c r="A156" s="1">
         <v>10661</v>
       </c>
@@ -42130,8 +42598,11 @@
       <c r="CJ156">
         <v>0</v>
       </c>
+      <c r="CK156">
+        <v>0</v>
+      </c>
     </row>
-    <row r="157" spans="1:88">
+    <row r="157" spans="1:89">
       <c r="A157" s="1">
         <v>10673</v>
       </c>
@@ -42396,8 +42867,11 @@
       <c r="CJ157">
         <v>0</v>
       </c>
+      <c r="CK157">
+        <v>0</v>
+      </c>
     </row>
-    <row r="158" spans="1:88">
+    <row r="158" spans="1:89">
       <c r="A158" s="1">
         <v>10705</v>
       </c>
@@ -42662,8 +43136,11 @@
       <c r="CJ158">
         <v>5</v>
       </c>
+      <c r="CK158">
+        <v>0</v>
+      </c>
     </row>
-    <row r="159" spans="1:88">
+    <row r="159" spans="1:89">
       <c r="A159" s="1">
         <v>10708</v>
       </c>
@@ -42928,8 +43405,11 @@
       <c r="CJ159">
         <v>0</v>
       </c>
+      <c r="CK159">
+        <v>0</v>
+      </c>
     </row>
-    <row r="160" spans="1:88">
+    <row r="160" spans="1:89">
       <c r="A160" s="1">
         <v>10734</v>
       </c>
@@ -43194,8 +43674,11 @@
       <c r="CJ160">
         <v>0</v>
       </c>
+      <c r="CK160">
+        <v>0</v>
+      </c>
     </row>
-    <row r="161" spans="1:88">
+    <row r="161" spans="1:89">
       <c r="A161" s="1">
         <v>10763</v>
       </c>
@@ -43460,8 +43943,11 @@
       <c r="CJ161">
         <v>0</v>
       </c>
+      <c r="CK161">
+        <v>0</v>
+      </c>
     </row>
-    <row r="162" spans="1:88">
+    <row r="162" spans="1:89">
       <c r="A162" s="1">
         <v>10773</v>
       </c>
@@ -43726,8 +44212,11 @@
       <c r="CJ162">
         <v>5</v>
       </c>
+      <c r="CK162">
+        <v>0</v>
+      </c>
     </row>
-    <row r="163" spans="1:88">
+    <row r="163" spans="1:89">
       <c r="A163" s="1">
         <v>10819</v>
       </c>
@@ -43992,8 +44481,11 @@
       <c r="CJ163">
         <v>3</v>
       </c>
+      <c r="CK163">
+        <v>0</v>
+      </c>
     </row>
-    <row r="164" spans="1:88">
+    <row r="164" spans="1:89">
       <c r="A164" s="1">
         <v>10844</v>
       </c>
@@ -44258,8 +44750,11 @@
       <c r="CJ164">
         <v>5</v>
       </c>
+      <c r="CK164">
+        <v>0</v>
+      </c>
     </row>
-    <row r="165" spans="1:88">
+    <row r="165" spans="1:89">
       <c r="A165" s="1">
         <v>10976</v>
       </c>
@@ -44524,8 +45019,11 @@
       <c r="CJ165">
         <v>5</v>
       </c>
+      <c r="CK165">
+        <v>0</v>
+      </c>
     </row>
-    <row r="166" spans="1:88">
+    <row r="166" spans="1:89">
       <c r="A166" s="1">
         <v>11086</v>
       </c>
@@ -44790,8 +45288,11 @@
       <c r="CJ166">
         <v>5</v>
       </c>
+      <c r="CK166">
+        <v>0</v>
+      </c>
     </row>
-    <row r="167" spans="1:88">
+    <row r="167" spans="1:89">
       <c r="A167" s="1">
         <v>11097</v>
       </c>
@@ -45056,8 +45557,11 @@
       <c r="CJ167">
         <v>0</v>
       </c>
+      <c r="CK167">
+        <v>0</v>
+      </c>
     </row>
-    <row r="168" spans="1:88">
+    <row r="168" spans="1:89">
       <c r="A168" s="1">
         <v>11104</v>
       </c>
@@ -45322,8 +45826,11 @@
       <c r="CJ168">
         <v>0</v>
       </c>
+      <c r="CK168">
+        <v>0</v>
+      </c>
     </row>
-    <row r="169" spans="1:88">
+    <row r="169" spans="1:89">
       <c r="A169" s="1">
         <v>11170</v>
       </c>
@@ -45588,8 +46095,11 @@
       <c r="CJ169">
         <v>2</v>
       </c>
+      <c r="CK169">
+        <v>0</v>
+      </c>
     </row>
-    <row r="170" spans="1:88">
+    <row r="170" spans="1:89">
       <c r="A170" s="1">
         <v>11200</v>
       </c>
@@ -45854,8 +46364,11 @@
       <c r="CJ170">
         <v>2</v>
       </c>
+      <c r="CK170">
+        <v>0</v>
+      </c>
     </row>
-    <row r="171" spans="1:88">
+    <row r="171" spans="1:89">
       <c r="A171" s="1">
         <v>11217</v>
       </c>
@@ -46120,8 +46633,11 @@
       <c r="CJ171">
         <v>6</v>
       </c>
+      <c r="CK171">
+        <v>0</v>
+      </c>
     </row>
-    <row r="172" spans="1:88">
+    <row r="172" spans="1:89">
       <c r="A172" s="1">
         <v>11253</v>
       </c>
@@ -46386,8 +46902,11 @@
       <c r="CJ172">
         <v>6</v>
       </c>
+      <c r="CK172">
+        <v>0</v>
+      </c>
     </row>
-    <row r="173" spans="1:88">
+    <row r="173" spans="1:89">
       <c r="A173" s="1">
         <v>11256</v>
       </c>
@@ -46652,8 +47171,11 @@
       <c r="CJ173">
         <v>0</v>
       </c>
+      <c r="CK173">
+        <v>0</v>
+      </c>
     </row>
-    <row r="174" spans="1:88">
+    <row r="174" spans="1:89">
       <c r="A174" s="1">
         <v>11379</v>
       </c>
@@ -46918,8 +47440,11 @@
       <c r="CJ174">
         <v>3</v>
       </c>
+      <c r="CK174">
+        <v>0</v>
+      </c>
     </row>
-    <row r="175" spans="1:88">
+    <row r="175" spans="1:89">
       <c r="A175" s="1">
         <v>11399</v>
       </c>
@@ -47183,6 +47708,9 @@
       </c>
       <c r="CJ175">
         <v>5</v>
+      </c>
+      <c r="CK175">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>